<commit_message>
Update design with dark theme and add new products
- Change background to dark grey
- Update header to dark blue gradient
- Add Streaming YouTube and Reading on a Kindle to product list

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Energy use of products.xlsx
+++ b/Energy use of products.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahritchie/Desktop/VSCode/energy-use-products/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahritchie/Desktop/data-projects/energy-use-products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB52B73-B559-004E-80C7-C5AF94C44FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3513A6-C217-7745-8D99-059FFAF5D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="840" windowWidth="27640" windowHeight="16460" xr2:uid="{E9F44B29-F67D-AA43-897E-E427581FB5C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Electricity" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>Product</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>Fridge-freezer</t>
+  </si>
+  <si>
+    <t>Streaming YouTube</t>
+  </si>
+  <si>
+    <t>Reading on a Kindle</t>
   </si>
 </sst>
 </file>
@@ -616,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A5542A6-C523-FF45-805D-8485BB9C76EC}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,7 +755,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:E17" si="1">B9*D9</f>
+        <f t="shared" ref="E9:E19" si="1">B9*D9</f>
         <v>70</v>
       </c>
     </row>
@@ -809,117 +815,130 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13" si="2">B13*D13</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>0.3</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15">
+        <v>0.2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15" si="3">B15*D15</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>1200</v>
       </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1">
         <f>1/60*5</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <v>2000</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>28</v>
       </c>
-      <c r="D16">
+      <c r="D18">
         <v>0.05</v>
       </c>
-      <c r="E16">
+      <c r="E18">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>2500</v>
       </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17">
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19">
         <v>0.5</v>
       </c>
-      <c r="E17">
+      <c r="E19">
         <f t="shared" si="1"/>
         <v>1250</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E20" s="2">
         <f>100*1000/365</f>
         <v>273.97260273972603</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>47</v>
-      </c>
-      <c r="E19" s="2">
-        <f>300*1000/365</f>
-        <v>821.91780821917803</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21">
-        <v>800</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21">
-        <v>0.16</v>
       </c>
       <c r="E21" s="2">
         <f>300*1000/365</f>
@@ -927,140 +946,141 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23">
+        <v>800</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23">
+        <v>0.16</v>
+      </c>
+      <c r="E23" s="2">
+        <f>300*1000/365</f>
+        <v>821.91780821917803</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>11</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <f>60*1000/100</f>
         <v>600</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24">
-        <v>1500</v>
-      </c>
-    </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25">
-        <v>2000</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25">
-        <v>0.16</v>
+        <v>26</v>
       </c>
       <c r="E25">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B27">
-        <v>1750</v>
+        <v>2000</v>
       </c>
       <c r="C27" t="s">
         <v>25</v>
       </c>
       <c r="D27">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="E27">
-        <f>B27*D27</f>
-        <v>140</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28">
-        <v>10000</v>
-      </c>
-      <c r="C28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28">
-        <v>0.16</v>
-      </c>
-      <c r="E28">
-        <f>B28*D28</f>
-        <v>1600</v>
+      <c r="A28" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B29">
-        <v>50</v>
+        <v>1750</v>
       </c>
       <c r="C29" t="s">
         <v>25</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0.08</v>
       </c>
       <c r="E29">
         <f>B29*D29</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30">
+        <v>10000</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30">
+        <v>0.16</v>
+      </c>
+      <c r="E30">
+        <f>B30*D30</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30">
-        <v>1000</v>
-      </c>
-      <c r="C30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31">
-        <v>3000</v>
-      </c>
       <c r="C31" t="s">
         <v>25</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f>B31*D31</f>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B32">
         <v>1000</v>
@@ -1068,17 +1088,10 @@
       <c r="C32" t="s">
         <v>25</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <f>B32*D32</f>
-        <v>1000</v>
-      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B33">
         <v>3000</v>
@@ -1086,76 +1099,105 @@
       <c r="C33" t="s">
         <v>25</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <f>B33*D33</f>
-        <v>3000</v>
-      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34">
+        <v>1000</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <f>B34*D34</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>3000</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <f>B35*D35</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B34">
+      <c r="B36">
         <v>4000</v>
       </c>
-      <c r="C34" t="s">
-        <v>25</v>
-      </c>
-      <c r="E34" s="2">
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="2">
         <f>'[1]Heating calculations'!B5*1000</f>
         <v>10958.904109589041</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C35" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="2">
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="2">
         <f>'[1]Heating calculations'!B10*1000</f>
         <v>32876.712328767127</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B37">
+      <c r="B39">
         <v>2.5</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>29</v>
       </c>
-      <c r="B38">
+      <c r="B40">
         <v>2.6</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>30</v>
       </c>
-      <c r="B39">
+      <c r="B41">
         <v>300</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update product data and wattage values
- Updated heating product wattages: Small desk heater (400W→750W), Electric heat pump Single room (500W→800W), Gas heating Single room (1000W→2700W)
- Added two new 3-bed house heating products: Electric heat pump (2250W) and Gas heating (7500W)
- Updated Excel and Word source documents with latest data

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Energy use of products.xlsx
+++ b/Energy use of products.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahritchie/Desktop/data-projects/energy-use-products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3513A6-C217-7745-8D99-059FFAF5D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E34291-5873-2340-B621-5C7A4B810033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="840" windowWidth="27640" windowHeight="16460" xr2:uid="{E9F44B29-F67D-AA43-897E-E427581FB5C3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{E9F44B29-F67D-AA43-897E-E427581FB5C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Electricity" sheetId="1" r:id="rId1"/>
+    <sheet name="Energy" sheetId="2" r:id="rId1"/>
+    <sheet name="Electricity" sheetId="1" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="75">
   <si>
     <t>Product</t>
   </si>
@@ -164,9 +165,6 @@
     <t>Hairdryer</t>
   </si>
   <si>
-    <t>Driving an e-bike</t>
-  </si>
-  <si>
     <t>Gaming consoles (Xbox)</t>
   </si>
   <si>
@@ -189,6 +187,84 @@
   </si>
   <si>
     <t>Reading on a Kindle</t>
+  </si>
+  <si>
+    <t>Using an e-bike</t>
+  </si>
+  <si>
+    <t>Driving a petrol car</t>
+  </si>
+  <si>
+    <t>Electric heat pump (Single room)</t>
+  </si>
+  <si>
+    <t>Electric induction hob (one ring)</t>
+  </si>
+  <si>
+    <t>Gas hob (one ring)</t>
+  </si>
+  <si>
+    <t>Air fryer</t>
+  </si>
+  <si>
+    <t>Gas heating (Single room)</t>
+  </si>
+  <si>
+    <t>Air conditioning (Single room)</t>
+  </si>
+  <si>
+    <t>Electric oven</t>
+  </si>
+  <si>
+    <t>Gas oven</t>
+  </si>
+  <si>
+    <t>Tumble dryer (vented or condenser)</t>
+  </si>
+  <si>
+    <t>Tumble dryer (heat pump)</t>
+  </si>
+  <si>
+    <t>Gas-powered shower</t>
+  </si>
+  <si>
+    <t>Gardening</t>
+  </si>
+  <si>
+    <t>Electric lawnmower</t>
+  </si>
+  <si>
+    <t>Petrol lawnmower</t>
+  </si>
+  <si>
+    <t>Laptop or efficient desktop</t>
+  </si>
+  <si>
+    <t>Gaming console (Xbox Series S)</t>
+  </si>
+  <si>
+    <t>Gaming console (Xbox Series X)</t>
+  </si>
+  <si>
+    <t>Full charge</t>
+  </si>
+  <si>
+    <t>Using an e-scooter</t>
+  </si>
+  <si>
+    <t>Driving an electric motorbike</t>
+  </si>
+  <si>
+    <t>Driving a petrol motorbike</t>
+  </si>
+  <si>
+    <t>Space heater</t>
+  </si>
+  <si>
+    <t>Gas heating (3-bed house)</t>
+  </si>
+  <si>
+    <t>Electric heat pump (3-bed house)</t>
   </si>
 </sst>
 </file>
@@ -621,11 +697,839 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B239A6D3-151C-6C42-AB20-47DEE8CAFF43}">
+  <dimension ref="A1:E55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>B3*D3</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>B4*D4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E20" si="0">B7*D7</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12">
+        <v>150</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12" si="1">B12*D12</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15">
+        <v>0.3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>2000</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18">
+        <v>0.05</v>
+      </c>
+      <c r="E18">
+        <f>B18*D18</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>1000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1">
+        <f>1/60*5</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>83.333333333333329</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20">
+        <v>2500</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>3000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21" si="2">B21*D21</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22">
+        <v>1000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="1">
+        <f>1/6</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" ref="E22:E23" si="3">B22*D22</f>
+        <v>166.66666666666666</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23">
+        <v>750</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="1">
+        <f>1/6</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="3"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24">
+        <v>1600</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="1">
+        <f>1/6</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" ref="E24" si="4">B24*D24</f>
+        <v>266.66666666666663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="2">
+        <f>300*1000/365</f>
+        <v>821.91780821917803</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28">
+        <v>750</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28">
+        <v>0.16</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" ref="E28" si="5">B28*D28</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33">
+        <v>2500</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33">
+        <v>0.16</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" ref="E33" si="6">B33*D33</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35">
+        <v>1750</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35">
+        <v>0.08</v>
+      </c>
+      <c r="E35">
+        <f>B35*D35</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <v>9500</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36">
+        <v>0.16</v>
+      </c>
+      <c r="E36">
+        <f>B36*D36</f>
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="2">
+        <f>B36/90%</f>
+        <v>10555.555555555555</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37">
+        <v>0.16</v>
+      </c>
+      <c r="E37" s="2">
+        <f>B37*D37</f>
+        <v>1688.8888888888887</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <v>50</v>
+      </c>
+      <c r="C38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <f>B38*D38</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39">
+        <v>750</v>
+      </c>
+      <c r="C39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <f>B39*D39</f>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40">
+        <v>1500</v>
+      </c>
+      <c r="C40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <f>B40*D40</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41">
+        <v>800</v>
+      </c>
+      <c r="C41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <f>B41*D41</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42">
+        <v>2250</v>
+      </c>
+      <c r="C42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <f>B42*D42</f>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43">
+        <v>2700</v>
+      </c>
+      <c r="C43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <f>B43*D43</f>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44">
+        <v>7500</v>
+      </c>
+      <c r="C44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <f>B44*D44</f>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45">
+        <v>1000</v>
+      </c>
+      <c r="C45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <f>B45*D45</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47">
+        <v>25</v>
+      </c>
+      <c r="C47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48">
+        <v>25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49">
+        <v>150</v>
+      </c>
+      <c r="C49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50">
+        <v>530</v>
+      </c>
+      <c r="C50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51">
+        <v>300</v>
+      </c>
+      <c r="C51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>1000</v>
+      </c>
+      <c r="C52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54">
+        <v>1500</v>
+      </c>
+      <c r="C54" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <f>B54*D54</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55">
+        <v>9000</v>
+      </c>
+      <c r="C55" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <f>B55*D55</f>
+        <v>9000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A5542A6-C523-FF45-805D-8485BB9C76EC}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -779,7 +1683,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11">
         <v>70</v>
@@ -815,7 +1719,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>20</v>
@@ -851,7 +1755,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>0.2</v>
@@ -929,7 +1833,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="2">
         <f>100*1000/365</f>
@@ -938,7 +1842,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="2">
         <f>300*1000/365</f>
@@ -947,12 +1851,12 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23">
         <v>800</v>
@@ -1004,7 +1908,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>2000</v>
@@ -1170,7 +2074,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B39">
         <v>2.5</v>

</xml_diff>